<commit_message>
fix relating to a record with no kemr_uuid variable in universal_client registration
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/universal_client-create.xlsx
+++ b/config/default/forms/contact/universal_client-create.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">choices!$A$1:$E$2055</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">choices!$A$1:$E$2055</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">choices!$A$1:$E$2055</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -703,7 +704,7 @@
     <t xml:space="preserve">Relation UUID</t>
   </si>
   <si>
-    <t xml:space="preserve">if(../relation/kemr_uuid !=’’,../relation/kemr_uuid,../relation/_id)</t>
+    <t xml:space="preserve">if(${kemr_uuid} !=’’,${kemr_uuid},${_id})</t>
   </si>
   <si>
     <t xml:space="preserve">relation_name</t>
@@ -7070,277 +7071,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="116">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
+  <dxfs count="86">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -8188,30 +7919,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y94"/>
+  <dimension ref="A1:Y65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A88" activeCellId="0" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.8877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.2448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.6785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="117.622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.1581632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.1275510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="176.658163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="58.9438775510204"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="70.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.5969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.5867346938775"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="121.852040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="48.8673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.8265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="183.051020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.1071428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="61.015306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.1071428571429"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="72.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="34.1071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10146,7 +9877,7 @@
       <c r="M79" s="3"/>
       <c r="N79" s="3"/>
     </row>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="17.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
         <v>18</v>
       </c>
@@ -10157,7 +9888,7 @@
         <v>211</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3" t="s">
@@ -10500,6 +10231,13 @@
       <c r="M94" s="19"/>
       <c r="N94" s="19"/>
     </row>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="B1">
     <cfRule type="cellIs" priority="2" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
@@ -11473,255 +11211,255 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="cellIs" priority="211" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+    <cfRule type="cellIs" priority="211" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" priority="212" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
+    <cfRule type="expression" priority="212" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
       <formula>COUNTIF($B$2:$B$1003,B47)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="213" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+    <cfRule type="expression" priority="213" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
       <formula>AND(A1 = "type", COUNTIF($A$1:$A$947, "begin group") = COUNTIF($A$1:$A$947, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="214" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+    <cfRule type="expression" priority="214" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
       <formula>ma(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$938, "begin group") = COUNTIF($A$1:$A$947, "end group")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="expression" priority="215" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
+    <cfRule type="expression" priority="215" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
       <formula>AND($A87="begin group", NOT($B87 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="cellIs" priority="216" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
+    <cfRule type="cellIs" priority="216" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I87">
-    <cfRule type="expression" priority="217" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71">
+    <cfRule type="expression" priority="217" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
       <formula>AND($I87 = "", $A87 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87">
-    <cfRule type="expression" priority="218" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
+    <cfRule type="expression" priority="218" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
       <formula>AND(AND(NOT($A87 = "end group"), NOT($A87 = "end repeat"), NOT($A87 = "")), $C87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87">
-    <cfRule type="expression" priority="219" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73">
+    <cfRule type="expression" priority="219" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
       <formula>AND(AND(NOT($A87 = "end group"), NOT($A87 = "end repeat"), NOT($A87 = "")), $B87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A87">
-    <cfRule type="cellIs" priority="220" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
+    <cfRule type="cellIs" priority="220" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87">
-    <cfRule type="expression" priority="221" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
+    <cfRule type="expression" priority="221" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
       <formula>AND(NOT($G87 = ""), $H87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="expression" priority="222" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
+    <cfRule type="expression" priority="222" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
       <formula>AND($A87="begin repeat", NOT($B87 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="expression" priority="223" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
+    <cfRule type="expression" priority="223" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
       <formula>AND($E87 = "", $A87 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="expression" priority="224" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
+    <cfRule type="expression" priority="224" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
       <formula>AND($A87="end repeat", $B87 = "", $C87 = "", $D87 = "", $E87 = "", $F87 = "", $G87 = "", $H87 = "", $E87 = "", $J87 = "", $K87 = "", $L87 = "", $M87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="expression" priority="225" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
+    <cfRule type="expression" priority="225" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
       <formula>AND($A87="end group", $B87 = "", $C87 = "", $D87 = "", $E87 = "", $F87 = "", $G87 = "", $H87 = "", $E87 = "", $J87 = "", $K87 = "", $L87 = "", $M87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="containsText" priority="226" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="80"/>
+    <cfRule type="containsText" priority="226" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88">
-    <cfRule type="expression" priority="227" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81">
+    <cfRule type="expression" priority="227" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
       <formula>AND($A87="begin group", NOT($B87 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88">
-    <cfRule type="cellIs" priority="228" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82">
+    <cfRule type="cellIs" priority="228" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I88">
-    <cfRule type="expression" priority="229" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83">
+    <cfRule type="expression" priority="229" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
       <formula>AND($I87 = "", $A87 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88">
-    <cfRule type="expression" priority="230" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84">
+    <cfRule type="expression" priority="230" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
       <formula>AND(AND(NOT($A87 = "end group"), NOT($A87 = "end repeat"), NOT($A87 = "")), $C87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="expression" priority="231" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
+    <cfRule type="expression" priority="231" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
       <formula>AND(AND(NOT($A87 = "end group"), NOT($A87 = "end repeat"), NOT($A87 = "")), $B87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="cellIs" priority="232" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86">
+    <cfRule type="cellIs" priority="232" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88">
-    <cfRule type="expression" priority="233" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86">
+    <cfRule type="expression" priority="233" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
       <formula>AND(NOT($G87 = ""), $H87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88">
-    <cfRule type="expression" priority="234" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
+    <cfRule type="expression" priority="234" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
       <formula>AND($A87="begin repeat", NOT($B87 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88">
-    <cfRule type="expression" priority="235" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
+    <cfRule type="expression" priority="235" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
       <formula>AND($E87 = "", $A87 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88">
-    <cfRule type="expression" priority="236" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89">
+    <cfRule type="expression" priority="236" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
       <formula>AND($A87="end repeat", $B87 = "", $C87 = "", $D87 = "", $E87 = "", $F87 = "", $G87 = "", $H87 = "", $E87 = "", $J87 = "", $K87 = "", $L87 = "", $M87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88">
-    <cfRule type="expression" priority="237" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
+    <cfRule type="expression" priority="237" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
       <formula>AND($A87="end group", $B87 = "", $C87 = "", $D87 = "", $E87 = "", $F87 = "", $G87 = "", $H87 = "", $E87 = "", $J87 = "", $K87 = "", $L87 = "", $M87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88">
-    <cfRule type="containsText" priority="238" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="91"/>
+    <cfRule type="containsText" priority="238" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76">
-    <cfRule type="containsText" priority="239" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="92"/>
+    <cfRule type="containsText" priority="239" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76">
-    <cfRule type="expression" priority="240" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93">
+    <cfRule type="expression" priority="240" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73">
       <formula>AND($A67="begin group", NOT($B67 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76">
-    <cfRule type="expression" priority="241" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94">
+    <cfRule type="expression" priority="241" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
       <formula>AND($A67="end group", $B67 = "", $C67 = "", $D67 = "", $E67 = "", $F67 = "", $G67 = "", $H67 = "", $I67 = "", $J67 = "", $K67 = "", $L67 = "", $M67 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76">
-    <cfRule type="cellIs" priority="242" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95">
+    <cfRule type="cellIs" priority="242" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76">
-    <cfRule type="expression" priority="243" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96">
+    <cfRule type="expression" priority="243" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
       <formula>AND($A67="begin repeat", NOT($B67 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76">
-    <cfRule type="expression" priority="244" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97">
+    <cfRule type="expression" priority="244" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
       <formula>AND($A67="end repeat", $B67 = "", $C67 = "", $D67 = "", $E67 = "", $F67 = "", $G67 = "", $H67 = "", $I67 = "", $J67 = "", $K67 = "", $L67 = "", $M67 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77">
-    <cfRule type="containsText" priority="245" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="98"/>
+    <cfRule type="containsText" priority="245" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="78"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77">
-    <cfRule type="expression" priority="246" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
+    <cfRule type="expression" priority="246" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
       <formula>AND($A47="begin group", NOT($B47 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77">
-    <cfRule type="expression" priority="247" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100">
+    <cfRule type="expression" priority="247" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
       <formula>AND($A47="end group", $B47 = "", $C47 = "", $D47 = "", $E47 = "", $F47 = "", $G47 = "", $H47 = "", $I47 = "", $J47 = "", $K47 = "", $L47 = "", $M47 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77">
-    <cfRule type="cellIs" priority="248" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101">
+    <cfRule type="cellIs" priority="248" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77">
-    <cfRule type="expression" priority="249" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
+    <cfRule type="expression" priority="249" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
       <formula>AND($A47="begin repeat", NOT($B47 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77">
-    <cfRule type="expression" priority="250" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
+    <cfRule type="expression" priority="250" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
       <formula>AND($A47="end repeat", $B47 = "", $C47 = "", $D47 = "", $E47 = "", $F47 = "", $G47 = "", $H47 = "", $I47 = "", $J47 = "", $K47 = "", $L47 = "", $M47 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78">
-    <cfRule type="containsText" priority="251" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="102"/>
+    <cfRule type="containsText" priority="251" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78">
-    <cfRule type="expression" priority="252" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
+    <cfRule type="expression" priority="252" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
       <formula>AND($A71="begin group", NOT($B71 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78">
-    <cfRule type="expression" priority="253" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
+    <cfRule type="expression" priority="253" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
       <formula>AND($A71="end group", $B71 = "", $C71 = "", $D71 = "", $E71 = "", $F71 = "", $G71 = "", $H71 = "", $I71 = "", $J71 = "", $K71 = "", $L71 = "", $M71 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78">
-    <cfRule type="cellIs" priority="254" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
+    <cfRule type="cellIs" priority="254" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78">
-    <cfRule type="expression" priority="255" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103">
+    <cfRule type="expression" priority="255" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81">
       <formula>AND($A71="begin repeat", NOT($B71 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78">
-    <cfRule type="expression" priority="256" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104">
+    <cfRule type="expression" priority="256" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82">
       <formula>AND($A71="end repeat", $B71 = "", $C71 = "", $D71 = "", $E71 = "", $F71 = "", $G71 = "", $H71 = "", $I71 = "", $J71 = "", $K71 = "", $L71 = "", $M71 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83">
-    <cfRule type="cellIs" priority="257" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105">
+    <cfRule type="cellIs" priority="257" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83">
-    <cfRule type="containsText" priority="258" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="106"/>
+    <cfRule type="containsText" priority="258" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="84"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83">
-    <cfRule type="expression" priority="259" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
+    <cfRule type="expression" priority="259" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
       <formula>AND($A83="begin group", NOT($B83 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83">
-    <cfRule type="expression" priority="260" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
+    <cfRule type="expression" priority="260" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
       <formula>AND($A83="end group", $B83 = "", $C83 = "", $D83 = "", $E83 = "", $F83 = "", $G83 = "", $H83 = "", $I83 = "", $J83 = "", $K83 = "", $L83 = "", $M83 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83">
-    <cfRule type="cellIs" priority="261" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
+    <cfRule type="cellIs" priority="261" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83">
-    <cfRule type="expression" priority="262" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
+    <cfRule type="expression" priority="262" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
       <formula>AND($A83="begin repeat", NOT($B83 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83">
-    <cfRule type="expression" priority="263" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
+    <cfRule type="expression" priority="263" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
       <formula>AND($A83="end repeat", $B83 = "", $C83 = "", $D83 = "", $E83 = "", $F83 = "", $G83 = "", $H83 = "", $I83 = "", $J83 = "", $K83 = "", $L83 = "", $M83 = "")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11759,10 +11497,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.75"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.3979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.9183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="34.1071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56441,9 +56179,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.7244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="34.1071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="34.1071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56478,7 +56216,7 @@
       </c>
       <c r="C2" s="37" t="n">
         <f aca="true">NOW()</f>
-        <v>44315.5315617494</v>
+        <v>44326.6943483928</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>2219</v>

</xml_diff>